<commit_message>
calculated sample 106 concentration after speed vacuum
</commit_message>
<xml_diff>
--- a/analyses/Virginica_MBDSeq_20180123/2018-01-23-MBDSeq-Labwork/2018-01-23-Virginica-MBDSeq-Labwork-Calculations.xlsx
+++ b/analyses/Virginica_MBDSeq_20180123/2018-01-23-MBDSeq-Labwork/2018-01-23-Virginica-MBDSeq-Labwork-Calculations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Documents/project-oyster-oa/analyses/Virginica_MBDSeq_20180123/2018-01-23-MBDSeq-Labwork/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10000" yWindow="460" windowWidth="15600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Sample</t>
   </si>
@@ -83,7 +83,13 @@
     <t>Volume for 25 ng/µL concentration (µL)</t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>New concentration (ng/µL)</t>
+  </si>
+  <si>
+    <t>106 Volume after speed vacuum (µL)</t>
+  </si>
+  <si>
+    <t>Volume water needed to dilute to 25 ng/µL (µL)</t>
   </si>
 </sst>
 </file>
@@ -127,13 +133,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,15 +421,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" customWidth="1"/>
     <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
@@ -1060,15 +1070,17 @@
         <f t="shared" si="1"/>
         <v>1.28</v>
       </c>
-      <c r="F10" t="s">
-        <v>18</v>
+      <c r="F10">
+        <f>(F15*F14)/25</f>
+        <v>51.2</v>
       </c>
       <c r="G10">
         <f>E10</f>
         <v>1.28</v>
       </c>
-      <c r="H10" t="s">
-        <v>18</v>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>51.2</v>
       </c>
       <c r="I10">
         <f t="shared" si="4"/>
@@ -1193,10 +1205,36 @@
         <v>8.2462400000000002</v>
       </c>
     </row>
+    <row r="14" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+      <c r="E14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+      <c r="E15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15">
+        <f>(B10*C10)/18</f>
+        <v>71.111111111111114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="E16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <f>F10-F14</f>
+        <v>33.200000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="K4 K7" formula="1"/>
+    <ignoredError sqref="K4 K7 F10" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added calculations necessary for elution
</commit_message>
<xml_diff>
--- a/analyses/Virginica_MBDSeq_20180123/2018-01-23-MBDSeq-Labwork/2018-01-23-Virginica-MBDSeq-Labwork-Calculations.xlsx
+++ b/analyses/Virginica_MBDSeq_20180123/2018-01-23-MBDSeq-Labwork/2018-01-23-Virginica-MBDSeq-Labwork-Calculations.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Day 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Day 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Sample</t>
   </si>
@@ -90,13 +91,19 @@
   </si>
   <si>
     <t>Volume water needed to dilute to 25 ng/µL (µL)</t>
+  </si>
+  <si>
+    <t>Volume water needed</t>
+  </si>
+  <si>
+    <t>Total Volume 1X Bind/Wash Buffer needed for removing non-captured DNA (µL)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,6 +115,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -421,10 +434,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,7 +452,7 @@
     <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,8 +507,11 @@
       <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>31</v>
       </c>
@@ -561,8 +580,12 @@
         <f>SUM(M2,N2,P2,Q2)</f>
         <v>832</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S2">
+        <f>500-100-H2</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>32</v>
       </c>
@@ -631,8 +654,12 @@
         <f t="shared" ref="R3:R11" si="11">SUM(M3,N3,P3,Q3)</f>
         <v>832</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S3">
+        <f t="shared" ref="S3:S11" si="12">500-100-H3</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>33</v>
       </c>
@@ -701,8 +728,12 @@
         <f t="shared" si="11"/>
         <v>772</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S4">
+        <f t="shared" si="12"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>35</v>
       </c>
@@ -771,8 +802,12 @@
         <f t="shared" si="11"/>
         <v>832</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S5">
+        <f t="shared" si="12"/>
+        <v>240.00000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>36</v>
       </c>
@@ -841,8 +876,12 @@
         <f t="shared" si="11"/>
         <v>832</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S6">
+        <f t="shared" si="12"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>103</v>
       </c>
@@ -911,8 +950,12 @@
         <f t="shared" si="11"/>
         <v>772</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S7">
+        <f t="shared" si="12"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>104</v>
       </c>
@@ -981,8 +1024,12 @@
         <f t="shared" si="11"/>
         <v>832</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S8">
+        <f t="shared" si="12"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>105</v>
       </c>
@@ -1020,7 +1067,7 @@
         <v>28</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K9:K11" si="12">100-I9</f>
+        <f t="shared" ref="K9:K11" si="13">100-I9</f>
         <v>60</v>
       </c>
       <c r="L9">
@@ -1051,8 +1098,12 @@
         <f t="shared" si="11"/>
         <v>832</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S9">
+        <f t="shared" si="12"/>
+        <v>240.00000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>106</v>
       </c>
@@ -1091,7 +1142,7 @@
         <v>8.9600000000000009</v>
       </c>
       <c r="K10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>87.2</v>
       </c>
       <c r="L10">
@@ -1122,8 +1173,12 @@
         <f t="shared" si="11"/>
         <v>878.24</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S10">
+        <f t="shared" si="12"/>
+        <v>348.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>108</v>
       </c>
@@ -1161,7 +1216,7 @@
         <v>28</v>
       </c>
       <c r="K11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>60</v>
       </c>
       <c r="L11">
@@ -1192,20 +1247,24 @@
         <f t="shared" si="11"/>
         <v>832</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S11">
+        <f t="shared" si="12"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="R12">
         <f>SUM(R2:R11)</f>
         <v>8246.24</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="R13">
         <f>R12*0.001</f>
         <v>8.2462400000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="E14" s="3" t="s">
         <v>19</v>
       </c>
@@ -1213,7 +1272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="E15" s="3" t="s">
         <v>18</v>
       </c>
@@ -1222,7 +1281,7 @@
         <v>71.111111111111114</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="E16" s="3" t="s">
         <v>20</v>
       </c>
@@ -1232,9 +1291,130 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="94" fitToWidth="2" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
     <ignoredError sqref="K4 K7 F10" formula="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="144" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <f>200*4</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B11" si="0">200*4</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>33</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>36</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>103</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>104</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>105</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>106</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>108</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <f>SUM(B2:B11)</f>
+        <v>8000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>